<commit_message>
init calcoloSpesaEnergetica e ConsumoEnergetico per HA
</commit_message>
<xml_diff>
--- a/doc/save_input_attributi.xlsx
+++ b/doc/save_input_attributi.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\save\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A45F71E-0420-4459-A4E0-DF67CC1D0225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9639EC-C7E7-4376-BF30-0C552F2A54B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D389C394-D6E6-4ED9-AA6C-2F68E59A05B4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{D389C394-D6E6-4ED9-AA6C-2F68E59A05B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="save_clusters" sheetId="3" r:id="rId2"/>
-    <sheet name="Foglio2" sheetId="4" r:id="rId3"/>
+    <sheet name="Foglio2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="153">
   <si>
     <t>table</t>
   </si>
@@ -701,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -749,9 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1072,23 +1069,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B11B50-7A68-4C69-AE29-910FA41495D2}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="1"/>
-    <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -1148,7 +1145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -1180,7 +1177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -1215,7 +1212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
@@ -1244,7 +1241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -1276,7 +1273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -1311,7 +1308,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -1369,7 +1366,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -1398,7 +1395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -1427,7 +1424,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -1456,7 +1453,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
@@ -1511,7 +1508,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
@@ -1537,7 +1534,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
         <v>86</v>
       </c>
@@ -1566,7 +1563,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>6</v>
       </c>
@@ -1594,7 +1591,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>130</v>
       </c>
@@ -1623,7 +1620,7 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -1651,7 +1648,7 @@
       </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -1680,7 +1677,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>130</v>
       </c>
@@ -1707,7 +1704,7 @@
       </c>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>130</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>130</v>
       </c>
@@ -1771,7 +1768,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>130</v>
       </c>
@@ -1800,7 +1797,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>130</v>
       </c>
@@ -1829,7 +1826,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>130</v>
       </c>
@@ -1860,8 +1857,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -1883,8 +1880,8 @@
       </c>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B31" s="31" t="s">
@@ -1912,8 +1909,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -1941,8 +1938,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -1968,8 +1965,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -1997,8 +1994,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B35" s="28" t="s">
@@ -2030,8 +2027,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B36" s="20" t="s">
@@ -2070,77 +2067,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2828560D-80C2-416C-821F-229AAE29C418}">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="35" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2444714-5E04-42BE-AF76-9671DFE53769}">
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="76.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -2151,12 +2092,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -2167,7 +2108,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -2178,7 +2119,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2189,7 +2130,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -2200,7 +2141,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -2211,7 +2152,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -2222,7 +2163,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -2233,7 +2174,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -2244,7 +2185,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -2255,7 +2196,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -2266,77 +2207,77 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="33" t="s">
         <v>148</v>
       </c>
       <c r="C18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="36" t="s">
+    <row r="19" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="34" t="s">
         <v>152</v>
       </c>
       <c r="C19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="34" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="33" t="s">
         <v>139</v>
       </c>
       <c r="C20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="33" t="s">
         <v>146</v>
       </c>
       <c r="C22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="35" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>151</v>
       </c>
       <c r="C23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="35" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>149</v>
       </c>
       <c r="C24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
         <v>150</v>
       </c>
       <c r="C25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="37"/>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2351,15 +2292,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D347722F4CD19B4AA30A301A73DC8334" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ace85805fe45a09026e851d5923a6fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="720644d8-bc67-4bc2-98e6-cafdf3eee657" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c73b4a14b4a9c94c6cca920ad0d090f5" ns3:_="">
     <xsd:import namespace="720644d8-bc67-4bc2-98e6-cafdf3eee657"/>
@@ -2491,6 +2423,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB33A76-A710-4FFA-A2A1-EAA7BAFE56EE}">
   <ds:schemaRefs>
@@ -2508,14 +2449,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E602BE76-2709-4AAF-A4DB-AB707C89CB87}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303BAA10-478C-40FD-864B-6DF0DE2E2B99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2531,4 +2464,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E602BE76-2709-4AAF-A4DB-AB707C89CB87}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modifiche excel campi tabelle
</commit_message>
<xml_diff>
--- a/doc/save_input_attributi.xlsx
+++ b/doc/save_input_attributi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\save\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EAF39B-D8F2-49F3-9175-F2CA968AA0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319FD601-0C33-4271-85EE-8797A5352617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2040" windowWidth="19200" windowHeight="9970" xr2:uid="{D389C394-D6E6-4ED9-AA6C-2F68E59A05B4}"/>
+    <workbookView xWindow="4620" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{D389C394-D6E6-4ED9-AA6C-2F68E59A05B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -691,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -743,6 +743,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1059,23 +1071,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B11B50-7A68-4C69-AE29-910FA41495D2}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="D15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="46.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -1135,7 +1147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -1167,7 +1179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -1263,7 +1275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -1327,7 +1339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -1385,7 +1397,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -1414,7 +1426,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -1443,7 +1455,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
@@ -1498,7 +1510,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>84</v>
       </c>
@@ -1553,7 +1565,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>6</v>
       </c>
@@ -1581,7 +1593,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -1610,7 +1622,7 @@
       </c>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -1638,7 +1650,7 @@
       </c>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -1667,7 +1679,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -1694,7 +1706,7 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>125</v>
       </c>
@@ -1727,7 +1739,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>125</v>
       </c>
@@ -1758,7 +1770,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>125</v>
       </c>
@@ -1787,7 +1799,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>125</v>
       </c>
@@ -1816,7 +1828,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>125</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>125</v>
       </c>
@@ -1870,7 +1882,7 @@
       </c>
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>125</v>
       </c>
@@ -1900,7 +1912,7 @@
       </c>
       <c r="L31" s="18"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>125</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>125</v>
       </c>
@@ -1956,7 +1968,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>125</v>
       </c>
@@ -1985,69 +1997,69 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="28">
+      <c r="E35" s="36">
+        <v>0</v>
+      </c>
+      <c r="F35" s="37">
         <v>4999</v>
       </c>
-      <c r="G35" s="28">
-        <v>0</v>
-      </c>
-      <c r="H35" s="4" t="s">
+      <c r="G35" s="37">
+        <v>0</v>
+      </c>
+      <c r="H35" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4" t="s">
+      <c r="I35" s="36"/>
+      <c r="J35" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="K35" s="29" t="s">
+      <c r="K35" s="38" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E36" s="20">
-        <v>0</v>
-      </c>
-      <c r="F36" s="21">
+      <c r="E36" s="40">
+        <v>0</v>
+      </c>
+      <c r="F36" s="41">
         <v>4999</v>
       </c>
-      <c r="G36" s="21">
-        <v>0</v>
-      </c>
-      <c r="H36" s="20" t="s">
+      <c r="G36" s="41">
+        <v>0</v>
+      </c>
+      <c r="H36" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20" t="s">
+      <c r="I36" s="40"/>
+      <c r="J36" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="K36" s="22" t="s">
+      <c r="K36" s="42" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2065,14 +2077,14 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="76.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -2083,12 +2095,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -2099,7 +2111,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2110,7 +2122,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2121,7 +2133,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -2132,7 +2144,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -2143,7 +2155,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -2165,7 +2177,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -2176,7 +2188,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -2187,7 +2199,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -2198,12 +2210,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
         <v>143</v>
       </c>
@@ -2211,7 +2223,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="31" t="s">
         <v>147</v>
       </c>
@@ -2219,7 +2231,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="30" t="s">
         <v>134</v>
       </c>
@@ -2227,7 +2239,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="30" t="s">
         <v>139</v>
       </c>
@@ -2235,7 +2247,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="30" t="s">
         <v>141</v>
       </c>
@@ -2243,7 +2255,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>146</v>
       </c>
@@ -2251,7 +2263,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>144</v>
       </c>
@@ -2259,7 +2271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>145</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" s="32"/>
     </row>
   </sheetData>
@@ -2277,9 +2289,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2415,26 +2430,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB33A76-A710-4FFA-A2A1-EAA7BAFE56EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E602BE76-2709-4AAF-A4DB-AB707C89CB87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="720644d8-bc67-4bc2-98e6-cafdf3eee657"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2458,9 +2462,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E602BE76-2709-4AAF-A4DB-AB707C89CB87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB33A76-A710-4FFA-A2A1-EAA7BAFE56EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="720644d8-bc67-4bc2-98e6-cafdf3eee657"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor for new db
</commit_message>
<xml_diff>
--- a/doc/save_input_attributi.xlsx
+++ b/doc/save_input_attributi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\save\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC88D95-0EA8-40BE-9943-7799E9BC5100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A249BD9-B6B2-4D42-8ECD-86A2EB160BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D389C394-D6E6-4ED9-AA6C-2F68E59A05B4}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D389C394-D6E6-4ED9-AA6C-2F68E59A05B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="167">
   <si>
     <t>table</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Fattore di conversione KWh TEP</t>
   </si>
   <si>
-    <t>tecnology</t>
-  </si>
-  <si>
     <t>Costo annuale gestione della zona omogenea</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
   </si>
   <si>
     <t>Ore accensione in dimmering</t>
-  </si>
-  <si>
-    <t>hour_online + hour_online_dimmering &lt; 5000</t>
   </si>
   <si>
     <t>save_has(TO_BE)</t>
@@ -518,6 +512,54 @@
   </si>
   <si>
     <t>???? Secondo noi è da togliere, non viene mai menzionata</t>
+  </si>
+  <si>
+    <t>hour_full_light + hour_dimmering_light &lt; 5000</t>
+  </si>
+  <si>
+    <t>lamp_tecnology</t>
+  </si>
+  <si>
+    <t>ref_has_is_id_cluster</t>
+  </si>
+  <si>
+    <t>Riferimento alla HAS ASIS associata</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>rappresenta per i cluster TOBE, il riferimento al cluster ASIS (1-to-n)</t>
+  </si>
+  <si>
+    <t>is_to_be_featured</t>
+  </si>
+  <si>
+    <t>Riferimento al cluster ASIS associato</t>
+  </si>
+  <si>
+    <t>Flag che indica la selezione</t>
+  </si>
+  <si>
+    <t>booleano (INT 0 o 1)</t>
+  </si>
+  <si>
+    <t>Indica se il cluster TOBE è selezionato per il cluster ASIS associato</t>
+  </si>
+  <si>
+    <t>save_clustersB32:K38</t>
+  </si>
+  <si>
+    <t>ref_has_is_id_ha</t>
+  </si>
+  <si>
+    <t>rappresenta per la HAS TOBE, il riferimento alla HAS ASIS (1-to-1)</t>
+  </si>
+  <si>
+    <t>is_ready</t>
+  </si>
+  <si>
+    <t>flag che indica che i campi sono pronti per il front-end</t>
   </si>
 </sst>
 </file>
@@ -700,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -727,7 +769,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -741,20 +782,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1069,25 +1124,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B11B50-7A68-4C69-AE29-910FA41495D2}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="1"/>
-    <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1116,9 +1171,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -1147,9 +1202,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>6</v>
@@ -1170,7 +1225,7 @@
         <v>100</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
@@ -1179,9 +1234,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>6</v>
@@ -1202,10 +1257,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>92</v>
       </c>
       <c r="J4" t="s">
         <v>29</v>
@@ -1214,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
@@ -1243,9 +1298,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>6</v>
@@ -1266,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -1275,9 +1330,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>6</v>
@@ -1298,10 +1353,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
         <v>29</v>
@@ -1310,9 +1365,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>6</v>
@@ -1339,9 +1394,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>6</v>
@@ -1368,9 +1423,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>6</v>
@@ -1397,9 +1452,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>6</v>
@@ -1426,9 +1481,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>6</v>
@@ -1452,21 +1507,21 @@
         <v>22</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
         <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1481,18 +1536,18 @@
         <v>42</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1507,18 +1562,18 @@
         <v>42</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1533,47 +1588,47 @@
         <v>29</v>
       </c>
       <c r="K15" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="35" t="s">
+      <c r="D16" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="J16" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>86</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>87</v>
       </c>
       <c r="E17" s="15">
         <v>0</v>
@@ -1590,476 +1645,575 @@
         <v>22</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="25"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="E21" s="36">
         <v>1</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F21" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="G21" s="36"/>
+      <c r="H21" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20">
+      <c r="E22" s="36">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F22" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="G20"/>
-      <c r="H20" t="s">
-        <v>85</v>
-      </c>
-      <c r="J20" t="s">
-        <v>77</v>
-      </c>
-      <c r="K20" s="11"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="G22" s="36"/>
+      <c r="H22" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>123</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D23" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="36">
+        <v>0</v>
+      </c>
+      <c r="F23" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="G23" s="36">
+        <v>0</v>
+      </c>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="K23" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="40">
+        <v>0</v>
+      </c>
+      <c r="F24" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>77</v>
-      </c>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="20" t="s">
+      <c r="G24" s="40">
+        <v>0</v>
+      </c>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" s="41"/>
+    </row>
+    <row r="25" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="40">
+        <v>1</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="42">
+        <v>1</v>
+      </c>
+      <c r="H25" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="I25" s="40"/>
+      <c r="J25" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="20">
+      <c r="D26" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="40">
+        <v>0</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="42">
+        <v>0</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="40">
+        <v>0</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="42">
+        <v>0</v>
+      </c>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="40">
+        <v>0</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="42">
+        <v>0</v>
+      </c>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="40">
+        <v>0</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="42">
+        <v>0</v>
+      </c>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="K30" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="K34" s="41"/>
+    </row>
+    <row r="35" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" s="40">
         <v>1</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F35" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="40">
         <v>1</v>
       </c>
-      <c r="H23" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="23" t="s">
+      <c r="F36" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="40">
+        <v>1</v>
+      </c>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" s="41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="40">
+        <v>0</v>
+      </c>
+      <c r="F37" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="40">
+        <v>0</v>
+      </c>
+      <c r="F38" s="40">
+        <v>100</v>
+      </c>
+      <c r="G38" s="40">
+        <v>0</v>
+      </c>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="K38" s="41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="40">
+        <v>0</v>
+      </c>
+      <c r="F39" s="42">
+        <v>4999</v>
+      </c>
+      <c r="G39" s="42">
+        <v>0</v>
+      </c>
+      <c r="H39" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="K39" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="24">
-        <v>0</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" s="25">
-        <v>0</v>
-      </c>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="28">
-        <v>0</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="28">
-        <v>0</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="20">
-        <v>0</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="21">
-        <v>0</v>
-      </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="18" t="s">
+    </row>
+    <row r="40" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="44">
+        <v>0</v>
+      </c>
+      <c r="F40" s="45">
+        <v>4999</v>
+      </c>
+      <c r="G40" s="45">
+        <v>0</v>
+      </c>
+      <c r="H40" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="E31" s="18">
-        <v>1</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K31" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="L31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="J32" t="s">
-        <v>56</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33"/>
-      <c r="J33" t="s">
-        <v>49</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
+      <c r="I40" s="44"/>
+      <c r="J40" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="K40" s="46" t="s">
         <v>100</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>29</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1">
-        <v>4999</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" t="s">
-        <v>98</v>
-      </c>
-      <c r="J35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0</v>
-      </c>
-      <c r="F36" s="16">
-        <v>4999</v>
-      </c>
-      <c r="G36" s="16">
-        <v>0</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2076,210 +2230,210 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="76.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="28" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
-        <v>139</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
-        <v>141</v>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="32"/>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2288,9 +2442,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2426,26 +2583,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB33A76-A710-4FFA-A2A1-EAA7BAFE56EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E602BE76-2709-4AAF-A4DB-AB707C89CB87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="720644d8-bc67-4bc2-98e6-cafdf3eee657"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2469,9 +2615,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E602BE76-2709-4AAF-A4DB-AB707C89CB87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CB33A76-A710-4FFA-A2A1-EAA7BAFE56EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="720644d8-bc67-4bc2-98e6-cafdf3eee657"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>